<commit_message>
changes metadata to match new LU table values and adds levels to metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/camp_markexisting_metadata.xlsx
+++ b/data-raw/metadata/camp_markexisting_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-knights-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D930D20F-9334-E241-B836-FCB2EC3D6CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1BC68EC-8569-FE4E-932B-4BEF97596080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="68">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -100,18 +100,6 @@
     <t>Primary key for record in this table</t>
   </si>
   <si>
-    <t>markTypeID</t>
-  </si>
-  <si>
-    <t>Code for the type of mark found on fish</t>
-  </si>
-  <si>
-    <t>markColorID</t>
-  </si>
-  <si>
-    <t>Code for the color of mark found on fish</t>
-  </si>
-  <si>
     <t>markPositionID</t>
   </si>
   <si>
@@ -133,30 +121,6 @@
     <t>attribute_name</t>
   </si>
   <si>
-    <t>Acoustic telemetry tag</t>
-  </si>
-  <si>
-    <t>Coded wire tag (CWT)</t>
-  </si>
-  <si>
-    <t>Elastomer</t>
-  </si>
-  <si>
-    <t>Fin clip</t>
-  </si>
-  <si>
-    <t>Floy tag</t>
-  </si>
-  <si>
-    <t>Freeze brand (bar)</t>
-  </si>
-  <si>
-    <t>Freeze brand (dot)</t>
-  </si>
-  <si>
-    <t>No marks or tags</t>
-  </si>
-  <si>
     <t>Not applicable (n/a)</t>
   </si>
   <si>
@@ -169,70 +133,10 @@
     <t>Other</t>
   </si>
   <si>
-    <t>Photonic Dye</t>
-  </si>
-  <si>
-    <t>Pigment / dye</t>
-  </si>
-  <si>
-    <t>PIT tag</t>
-  </si>
-  <si>
-    <t>Radio telemetry tag</t>
-  </si>
-  <si>
     <t>See Comments</t>
   </si>
   <si>
     <t>Unknown</t>
-  </si>
-  <si>
-    <t>Black</t>
-  </si>
-  <si>
-    <t>Blue</t>
-  </si>
-  <si>
-    <t>Brown</t>
-  </si>
-  <si>
-    <t>Cobalt blue</t>
-  </si>
-  <si>
-    <t>Dark blue</t>
-  </si>
-  <si>
-    <t>Flourescent blue</t>
-  </si>
-  <si>
-    <t>Flourescent green</t>
-  </si>
-  <si>
-    <t>Flourescent red</t>
-  </si>
-  <si>
-    <t>Green</t>
-  </si>
-  <si>
-    <t>Magenta</t>
-  </si>
-  <si>
-    <t>Orange</t>
-  </si>
-  <si>
-    <t>Pink</t>
-  </si>
-  <si>
-    <t>Purple / Violet</t>
-  </si>
-  <si>
-    <t>Red</t>
-  </si>
-  <si>
-    <t>White</t>
-  </si>
-  <si>
-    <t>Yellow</t>
   </si>
   <si>
     <t>Adipose fin</t>
@@ -314,6 +218,20 @@
   </si>
   <si>
     <t>Knights Landing RST Program</t>
+  </si>
+  <si>
+    <t>markType</t>
+  </si>
+  <si>
+    <t>markColor</t>
+  </si>
+  <si>
+    <t>Type of mark found on fish. Levels = c("No marks or tags", "Fin clip", "Pigment / dye", "Elastomer", 
+"Acoustic telemetry tag", "Coded wire tag (CWT)")</t>
+  </si>
+  <si>
+    <t>Color of mark found on fish. Levles = c("Not applicable (n/a)", "Brown", "Blue", "Purple / Violet", 
+"Orange", "Pink", "Green", "Not recorded")</t>
   </si>
 </sst>
 </file>
@@ -639,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1008"/>
+  <dimension ref="A1:Z1006"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -850,9 +768,9 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="2"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="11"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -882,13 +800,13 @@
         <v>16</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="6"/>
+      <c r="J6" s="3"/>
       <c r="K6" s="2"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
@@ -908,10 +826,10 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>28</v>
+        <v>64</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>15</v>
@@ -920,15 +838,15 @@
         <v>16</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="3"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="11"/>
       <c r="M7" s="3"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -946,10 +864,10 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>15</v>
@@ -964,7 +882,7 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="3"/>
+      <c r="J8" s="6"/>
       <c r="K8" s="2"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -982,7 +900,7 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
     </row>
-    <row r="9" spans="1:26" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1010,7 +928,7 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1066,7 +984,7 @@
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
     </row>
-    <row r="12" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1935,7 +1853,7 @@
       <c r="Z42" s="1"/>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="4"/>
+      <c r="A43" s="16"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="2"/>
@@ -1963,7 +1881,7 @@
       <c r="Z43" s="1"/>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="4"/>
+      <c r="A44" s="17"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="2"/>
@@ -2047,7 +1965,7 @@
       <c r="Z46" s="1"/>
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="16"/>
+      <c r="A47" s="4"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="2"/>
@@ -2075,7 +1993,7 @@
       <c r="Z47" s="1"/>
     </row>
     <row r="48" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="17"/>
+      <c r="A48" s="4"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="2"/>
@@ -2999,7 +2917,7 @@
       <c r="Z80" s="1"/>
     </row>
     <row r="81" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="4"/>
+      <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="2"/>
@@ -3027,7 +2945,7 @@
       <c r="Z81" s="1"/>
     </row>
     <row r="82" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="4"/>
+      <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="2"/>
@@ -28926,78 +28844,22 @@
       <c r="Y1006" s="1"/>
       <c r="Z1006" s="1"/>
     </row>
-    <row r="1007" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1007" s="1"/>
-      <c r="B1007" s="1"/>
-      <c r="C1007" s="1"/>
-      <c r="D1007" s="2"/>
-      <c r="E1007" s="1"/>
-      <c r="F1007" s="3"/>
-      <c r="G1007" s="3"/>
-      <c r="H1007" s="3"/>
-      <c r="I1007" s="2"/>
-      <c r="J1007" s="3"/>
-      <c r="K1007" s="2"/>
-      <c r="L1007" s="3"/>
-      <c r="M1007" s="3"/>
-      <c r="N1007" s="1"/>
-      <c r="O1007" s="1"/>
-      <c r="P1007" s="1"/>
-      <c r="Q1007" s="1"/>
-      <c r="R1007" s="1"/>
-      <c r="S1007" s="1"/>
-      <c r="T1007" s="1"/>
-      <c r="U1007" s="1"/>
-      <c r="V1007" s="1"/>
-      <c r="W1007" s="1"/>
-      <c r="X1007" s="1"/>
-      <c r="Y1007" s="1"/>
-      <c r="Z1007" s="1"/>
-    </row>
-    <row r="1008" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1008" s="1"/>
-      <c r="B1008" s="1"/>
-      <c r="C1008" s="1"/>
-      <c r="D1008" s="2"/>
-      <c r="E1008" s="1"/>
-      <c r="F1008" s="3"/>
-      <c r="G1008" s="3"/>
-      <c r="H1008" s="3"/>
-      <c r="I1008" s="2"/>
-      <c r="J1008" s="3"/>
-      <c r="K1008" s="2"/>
-      <c r="L1008" s="3"/>
-      <c r="M1008" s="3"/>
-      <c r="N1008" s="1"/>
-      <c r="O1008" s="1"/>
-      <c r="P1008" s="1"/>
-      <c r="Q1008" s="1"/>
-      <c r="R1008" s="1"/>
-      <c r="S1008" s="1"/>
-      <c r="T1008" s="1"/>
-      <c r="U1008" s="1"/>
-      <c r="V1008" s="1"/>
-      <c r="W1008" s="1"/>
-      <c r="X1008" s="1"/>
-      <c r="Y1008" s="1"/>
-      <c r="Z1008" s="1"/>
-    </row>
   </sheetData>
   <mergeCells count="2">
+    <mergeCell ref="A43:A44"/>
     <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A47:A48"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E1:E1008" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C63:C1006 C1:C4 C5:C51" xr:uid="{00000000-0002-0000-0000-000002000000}">
+      <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E1:E4 E5:E1006" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F1:F1008" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F1:F4 F5:F1006" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C1:C53 C65:C1008" xr:uid="{00000000-0002-0000-0000-000002000000}">
-      <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H1:H1008" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H1:H4 H5:H1006" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>
@@ -29008,10 +28870,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z960"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A3" sqref="A3:XFD42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -29024,13 +28886,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
@@ -29061,7 +28923,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>13</v>
@@ -29092,10 +28954,10 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>24</v>
@@ -29105,7 +28967,7 @@
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
       <c r="H3" s="14"/>
-      <c r="I3" s="15"/>
+      <c r="I3" s="14"/>
       <c r="J3" s="14"/>
       <c r="K3" s="14"/>
       <c r="L3" s="14"/>
@@ -29126,10 +28988,10 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>24</v>
@@ -29139,7 +29001,7 @@
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
-      <c r="I4" s="15"/>
+      <c r="I4" s="14"/>
       <c r="J4" s="14"/>
       <c r="K4" s="14"/>
       <c r="L4" s="14"/>
@@ -29160,10 +29022,10 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>24</v>
@@ -29194,10 +29056,10 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>24</v>
@@ -29228,10 +29090,10 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>24</v>
@@ -29260,12 +29122,12 @@
       <c r="Y7" s="14"/>
       <c r="Z7" s="14"/>
     </row>
-    <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>24</v>
@@ -29296,10 +29158,10 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>24</v>
@@ -29330,10 +29192,10 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>24</v>
@@ -29364,10 +29226,10 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14">
-        <v>252</v>
+        <v>25</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>24</v>
@@ -29398,10 +29260,10 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14">
-        <v>251</v>
+        <v>14</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>24</v>
@@ -29432,10 +29294,10 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14">
-        <v>255</v>
+        <v>26</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>24</v>
@@ -29466,10 +29328,10 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="14">
-        <v>250</v>
+        <v>22</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>24</v>
@@ -29500,10 +29362,10 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>24</v>
@@ -29534,10 +29396,10 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="14">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>24</v>
@@ -29568,10 +29430,10 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="14">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>24</v>
@@ -29602,10 +29464,10 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="14">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>24</v>
@@ -29636,10 +29498,10 @@
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="14">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="C19" s="15" t="s">
         <v>24</v>
@@ -29670,10 +29532,10 @@
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="14">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>24</v>
@@ -29704,13 +29566,13 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="14">
-        <v>7</v>
+        <v>255</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
@@ -29738,13 +29600,13 @@
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="14">
-        <v>2</v>
+        <v>250</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
@@ -29772,13 +29634,13 @@
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="14">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
@@ -29806,13 +29668,13 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="14">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
@@ -29840,13 +29702,13 @@
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="14">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
@@ -29874,13 +29736,13 @@
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="14">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
@@ -29908,13 +29770,13 @@
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="14">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
@@ -29942,13 +29804,13 @@
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="14">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
@@ -29976,13 +29838,13 @@
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="14">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
@@ -30010,13 +29872,13 @@
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="14">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D30" s="14"/>
       <c r="E30" s="14"/>
@@ -30044,13 +29906,13 @@
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="14">
-        <v>252</v>
+        <v>19</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D31" s="14"/>
       <c r="E31" s="14"/>
@@ -30078,13 +29940,13 @@
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="14">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D32" s="14"/>
       <c r="E32" s="14"/>
@@ -30112,13 +29974,13 @@
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="14">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D33" s="14"/>
       <c r="E33" s="14"/>
@@ -30146,13 +30008,13 @@
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="14">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D34" s="14"/>
       <c r="E34" s="14"/>
@@ -30179,15 +30041,9 @@
       <c r="Z34" s="14"/>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="14">
-        <v>250</v>
-      </c>
-      <c r="B35" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>26</v>
-      </c>
+      <c r="A35" s="12"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="12"/>
       <c r="D35" s="14"/>
       <c r="E35" s="14"/>
       <c r="F35" s="14"/>
@@ -30213,15 +30069,9 @@
       <c r="Z35" s="14"/>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="14">
-        <v>10</v>
-      </c>
-      <c r="B36" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="C36" s="15" t="s">
-        <v>26</v>
-      </c>
+      <c r="A36" s="12"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="12"/>
       <c r="D36" s="14"/>
       <c r="E36" s="14"/>
       <c r="F36" s="14"/>
@@ -30247,15 +30097,9 @@
       <c r="Z36" s="14"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="14">
-        <v>11</v>
-      </c>
-      <c r="B37" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>26</v>
-      </c>
+      <c r="A37" s="12"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="12"/>
       <c r="D37" s="14"/>
       <c r="E37" s="14"/>
       <c r="F37" s="14"/>
@@ -30281,15 +30125,9 @@
       <c r="Z37" s="14"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="14">
-        <v>14</v>
-      </c>
-      <c r="B38" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="C38" s="15" t="s">
-        <v>26</v>
-      </c>
+      <c r="A38" s="12"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="12"/>
       <c r="D38" s="14"/>
       <c r="E38" s="14"/>
       <c r="F38" s="14"/>
@@ -30315,15 +30153,9 @@
       <c r="Z38" s="14"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="14">
-        <v>254</v>
-      </c>
-      <c r="B39" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>26</v>
-      </c>
+      <c r="A39" s="12"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="12"/>
       <c r="D39" s="14"/>
       <c r="E39" s="14"/>
       <c r="F39" s="14"/>
@@ -30349,15 +30181,9 @@
       <c r="Z39" s="14"/>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="14">
-        <v>253</v>
-      </c>
-      <c r="B40" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C40" s="15" t="s">
-        <v>26</v>
-      </c>
+      <c r="A40" s="12"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="12"/>
       <c r="D40" s="14"/>
       <c r="E40" s="14"/>
       <c r="F40" s="14"/>
@@ -30383,15 +30209,9 @@
       <c r="Z40" s="14"/>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="14">
-        <v>8</v>
-      </c>
-      <c r="B41" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="C41" s="15" t="s">
-        <v>26</v>
-      </c>
+      <c r="A41" s="12"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="12"/>
       <c r="D41" s="14"/>
       <c r="E41" s="14"/>
       <c r="F41" s="14"/>
@@ -30417,15 +30237,9 @@
       <c r="Z41" s="14"/>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="14">
-        <v>12</v>
-      </c>
-      <c r="B42" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="C42" s="15" t="s">
-        <v>26</v>
-      </c>
+      <c r="A42" s="12"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="12"/>
       <c r="D42" s="14"/>
       <c r="E42" s="14"/>
       <c r="F42" s="14"/>
@@ -30451,15 +30265,9 @@
       <c r="Z42" s="14"/>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="14">
-        <v>1</v>
-      </c>
-      <c r="B43" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="C43" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="A43" s="12"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="12"/>
       <c r="D43" s="14"/>
       <c r="E43" s="14"/>
       <c r="F43" s="14"/>
@@ -30485,15 +30293,9 @@
       <c r="Z43" s="14"/>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="14">
-        <v>6</v>
-      </c>
-      <c r="B44" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="C44" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="A44" s="12"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="12"/>
       <c r="D44" s="14"/>
       <c r="E44" s="14"/>
       <c r="F44" s="14"/>
@@ -30519,15 +30321,9 @@
       <c r="Z44" s="14"/>
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="14">
-        <v>5</v>
-      </c>
-      <c r="B45" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="C45" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="A45" s="12"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="12"/>
       <c r="D45" s="14"/>
       <c r="E45" s="14"/>
       <c r="F45" s="14"/>
@@ -30553,15 +30349,9 @@
       <c r="Z45" s="14"/>
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="14">
-        <v>4</v>
-      </c>
-      <c r="B46" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="C46" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="A46" s="12"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="12"/>
       <c r="D46" s="14"/>
       <c r="E46" s="14"/>
       <c r="F46" s="14"/>
@@ -30587,15 +30377,9 @@
       <c r="Z46" s="14"/>
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="14">
-        <v>3</v>
-      </c>
-      <c r="B47" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="C47" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="A47" s="12"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="12"/>
       <c r="D47" s="14"/>
       <c r="E47" s="14"/>
       <c r="F47" s="14"/>
@@ -30621,15 +30405,9 @@
       <c r="Z47" s="14"/>
     </row>
     <row r="48" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="14">
-        <v>2</v>
-      </c>
-      <c r="B48" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="C48" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="A48" s="12"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="12"/>
       <c r="D48" s="14"/>
       <c r="E48" s="14"/>
       <c r="F48" s="14"/>
@@ -30655,15 +30433,9 @@
       <c r="Z48" s="14"/>
     </row>
     <row r="49" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="14">
-        <v>23</v>
-      </c>
-      <c r="B49" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="C49" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="A49" s="12"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="12"/>
       <c r="D49" s="14"/>
       <c r="E49" s="14"/>
       <c r="F49" s="14"/>
@@ -30689,15 +30461,9 @@
       <c r="Z49" s="14"/>
     </row>
     <row r="50" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="14">
-        <v>24</v>
-      </c>
-      <c r="B50" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="C50" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="A50" s="12"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="12"/>
       <c r="D50" s="14"/>
       <c r="E50" s="14"/>
       <c r="F50" s="14"/>
@@ -30723,15 +30489,9 @@
       <c r="Z50" s="14"/>
     </row>
     <row r="51" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="14">
-        <v>25</v>
-      </c>
-      <c r="B51" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="C51" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="A51" s="12"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="12"/>
       <c r="D51" s="14"/>
       <c r="E51" s="14"/>
       <c r="F51" s="14"/>
@@ -30757,15 +30517,9 @@
       <c r="Z51" s="14"/>
     </row>
     <row r="52" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="14">
-        <v>14</v>
-      </c>
-      <c r="B52" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="C52" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="A52" s="12"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="12"/>
       <c r="D52" s="14"/>
       <c r="E52" s="14"/>
       <c r="F52" s="14"/>
@@ -30791,15 +30545,9 @@
       <c r="Z52" s="14"/>
     </row>
     <row r="53" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="14">
-        <v>26</v>
-      </c>
-      <c r="B53" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="C53" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="A53" s="12"/>
+      <c r="B53" s="13"/>
+      <c r="C53" s="12"/>
       <c r="D53" s="14"/>
       <c r="E53" s="14"/>
       <c r="F53" s="14"/>
@@ -30825,15 +30573,9 @@
       <c r="Z53" s="14"/>
     </row>
     <row r="54" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="14">
-        <v>22</v>
-      </c>
-      <c r="B54" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C54" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="A54" s="12"/>
+      <c r="B54" s="13"/>
+      <c r="C54" s="12"/>
       <c r="D54" s="14"/>
       <c r="E54" s="14"/>
       <c r="F54" s="14"/>
@@ -30859,15 +30601,9 @@
       <c r="Z54" s="14"/>
     </row>
     <row r="55" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="14">
-        <v>15</v>
-      </c>
-      <c r="B55" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C55" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="A55" s="12"/>
+      <c r="B55" s="13"/>
+      <c r="C55" s="12"/>
       <c r="D55" s="14"/>
       <c r="E55" s="14"/>
       <c r="F55" s="14"/>
@@ -30893,15 +30629,9 @@
       <c r="Z55" s="14"/>
     </row>
     <row r="56" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="14">
-        <v>17</v>
-      </c>
-      <c r="B56" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="C56" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="A56" s="12"/>
+      <c r="B56" s="13"/>
+      <c r="C56" s="12"/>
       <c r="D56" s="14"/>
       <c r="E56" s="14"/>
       <c r="F56" s="14"/>
@@ -30927,15 +30657,9 @@
       <c r="Z56" s="14"/>
     </row>
     <row r="57" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="14">
-        <v>16</v>
-      </c>
-      <c r="B57" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="C57" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="A57" s="12"/>
+      <c r="B57" s="13"/>
+      <c r="C57" s="12"/>
       <c r="D57" s="14"/>
       <c r="E57" s="14"/>
       <c r="F57" s="14"/>
@@ -30961,15 +30685,9 @@
       <c r="Z57" s="14"/>
     </row>
     <row r="58" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="14">
-        <v>13</v>
-      </c>
-      <c r="B58" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="C58" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="A58" s="12"/>
+      <c r="B58" s="13"/>
+      <c r="C58" s="12"/>
       <c r="D58" s="14"/>
       <c r="E58" s="14"/>
       <c r="F58" s="14"/>
@@ -30995,15 +30713,9 @@
       <c r="Z58" s="14"/>
     </row>
     <row r="59" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="14">
-        <v>252</v>
-      </c>
-      <c r="B59" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C59" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="A59" s="12"/>
+      <c r="B59" s="13"/>
+      <c r="C59" s="12"/>
       <c r="D59" s="14"/>
       <c r="E59" s="14"/>
       <c r="F59" s="14"/>
@@ -31029,15 +30741,9 @@
       <c r="Z59" s="14"/>
     </row>
     <row r="60" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="14">
-        <v>251</v>
-      </c>
-      <c r="B60" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="C60" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="A60" s="12"/>
+      <c r="B60" s="13"/>
+      <c r="C60" s="12"/>
       <c r="D60" s="14"/>
       <c r="E60" s="14"/>
       <c r="F60" s="14"/>
@@ -31063,15 +30769,9 @@
       <c r="Z60" s="14"/>
     </row>
     <row r="61" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="14">
-        <v>255</v>
-      </c>
-      <c r="B61" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C61" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="A61" s="12"/>
+      <c r="B61" s="13"/>
+      <c r="C61" s="12"/>
       <c r="D61" s="14"/>
       <c r="E61" s="14"/>
       <c r="F61" s="14"/>
@@ -31097,15 +30797,9 @@
       <c r="Z61" s="14"/>
     </row>
     <row r="62" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="14">
-        <v>250</v>
-      </c>
-      <c r="B62" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C62" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="A62" s="12"/>
+      <c r="B62" s="13"/>
+      <c r="C62" s="12"/>
       <c r="D62" s="14"/>
       <c r="E62" s="14"/>
       <c r="F62" s="14"/>
@@ -31131,15 +30825,9 @@
       <c r="Z62" s="14"/>
     </row>
     <row r="63" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="14">
-        <v>10</v>
-      </c>
-      <c r="B63" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="C63" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="A63" s="12"/>
+      <c r="B63" s="13"/>
+      <c r="C63" s="12"/>
       <c r="D63" s="14"/>
       <c r="E63" s="14"/>
       <c r="F63" s="14"/>
@@ -31165,15 +30853,9 @@
       <c r="Z63" s="14"/>
     </row>
     <row r="64" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="14">
-        <v>11</v>
-      </c>
-      <c r="B64" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="C64" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="A64" s="12"/>
+      <c r="B64" s="13"/>
+      <c r="C64" s="12"/>
       <c r="D64" s="14"/>
       <c r="E64" s="14"/>
       <c r="F64" s="14"/>
@@ -31199,15 +30881,9 @@
       <c r="Z64" s="14"/>
     </row>
     <row r="65" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="14">
-        <v>12</v>
-      </c>
-      <c r="B65" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="C65" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="A65" s="12"/>
+      <c r="B65" s="13"/>
+      <c r="C65" s="12"/>
       <c r="D65" s="14"/>
       <c r="E65" s="14"/>
       <c r="F65" s="14"/>
@@ -31233,15 +30909,9 @@
       <c r="Z65" s="14"/>
     </row>
     <row r="66" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="14">
-        <v>7</v>
-      </c>
-      <c r="B66" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="C66" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="A66" s="12"/>
+      <c r="B66" s="13"/>
+      <c r="C66" s="12"/>
       <c r="D66" s="14"/>
       <c r="E66" s="14"/>
       <c r="F66" s="14"/>
@@ -31267,15 +30937,9 @@
       <c r="Z66" s="14"/>
     </row>
     <row r="67" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="14">
-        <v>8</v>
-      </c>
-      <c r="B67" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="C67" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="A67" s="12"/>
+      <c r="B67" s="13"/>
+      <c r="C67" s="12"/>
       <c r="D67" s="14"/>
       <c r="E67" s="14"/>
       <c r="F67" s="14"/>
@@ -31301,15 +30965,9 @@
       <c r="Z67" s="14"/>
     </row>
     <row r="68" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="14">
-        <v>9</v>
-      </c>
-      <c r="B68" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="C68" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="A68" s="12"/>
+      <c r="B68" s="13"/>
+      <c r="C68" s="12"/>
       <c r="D68" s="14"/>
       <c r="E68" s="14"/>
       <c r="F68" s="14"/>
@@ -31335,15 +30993,9 @@
       <c r="Z68" s="14"/>
     </row>
     <row r="69" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="14">
-        <v>18</v>
-      </c>
-      <c r="B69" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="C69" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="A69" s="12"/>
+      <c r="B69" s="13"/>
+      <c r="C69" s="12"/>
       <c r="D69" s="14"/>
       <c r="E69" s="14"/>
       <c r="F69" s="14"/>
@@ -31369,15 +31021,9 @@
       <c r="Z69" s="14"/>
     </row>
     <row r="70" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="14">
-        <v>20</v>
-      </c>
-      <c r="B70" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="C70" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="A70" s="12"/>
+      <c r="B70" s="13"/>
+      <c r="C70" s="12"/>
       <c r="D70" s="14"/>
       <c r="E70" s="14"/>
       <c r="F70" s="14"/>
@@ -31403,15 +31049,9 @@
       <c r="Z70" s="14"/>
     </row>
     <row r="71" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="14">
-        <v>19</v>
-      </c>
-      <c r="B71" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="C71" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="A71" s="12"/>
+      <c r="B71" s="13"/>
+      <c r="C71" s="12"/>
       <c r="D71" s="14"/>
       <c r="E71" s="14"/>
       <c r="F71" s="14"/>
@@ -31437,15 +31077,9 @@
       <c r="Z71" s="14"/>
     </row>
     <row r="72" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="14">
-        <v>254</v>
-      </c>
-      <c r="B72" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="C72" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="A72" s="12"/>
+      <c r="B72" s="13"/>
+      <c r="C72" s="12"/>
       <c r="D72" s="14"/>
       <c r="E72" s="14"/>
       <c r="F72" s="14"/>
@@ -31471,15 +31105,9 @@
       <c r="Z72" s="14"/>
     </row>
     <row r="73" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="14">
-        <v>253</v>
-      </c>
-      <c r="B73" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C73" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="A73" s="12"/>
+      <c r="B73" s="13"/>
+      <c r="C73" s="12"/>
       <c r="D73" s="14"/>
       <c r="E73" s="14"/>
       <c r="F73" s="14"/>
@@ -31505,15 +31133,9 @@
       <c r="Z73" s="14"/>
     </row>
     <row r="74" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="14">
-        <v>21</v>
-      </c>
-      <c r="B74" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="C74" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="A74" s="12"/>
+      <c r="B74" s="13"/>
+      <c r="C74" s="12"/>
       <c r="D74" s="14"/>
       <c r="E74" s="14"/>
       <c r="F74" s="14"/>
@@ -56346,1126 +55968,6 @@
       <c r="Y960" s="14"/>
       <c r="Z960" s="14"/>
     </row>
-    <row r="961" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A961" s="12"/>
-      <c r="B961" s="13"/>
-      <c r="C961" s="12"/>
-      <c r="D961" s="14"/>
-      <c r="E961" s="14"/>
-      <c r="F961" s="14"/>
-      <c r="G961" s="14"/>
-      <c r="H961" s="14"/>
-      <c r="I961" s="14"/>
-      <c r="J961" s="14"/>
-      <c r="K961" s="14"/>
-      <c r="L961" s="14"/>
-      <c r="M961" s="14"/>
-      <c r="N961" s="14"/>
-      <c r="O961" s="14"/>
-      <c r="P961" s="14"/>
-      <c r="Q961" s="14"/>
-      <c r="R961" s="14"/>
-      <c r="S961" s="14"/>
-      <c r="T961" s="14"/>
-      <c r="U961" s="14"/>
-      <c r="V961" s="14"/>
-      <c r="W961" s="14"/>
-      <c r="X961" s="14"/>
-      <c r="Y961" s="14"/>
-      <c r="Z961" s="14"/>
-    </row>
-    <row r="962" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A962" s="12"/>
-      <c r="B962" s="13"/>
-      <c r="C962" s="12"/>
-      <c r="D962" s="14"/>
-      <c r="E962" s="14"/>
-      <c r="F962" s="14"/>
-      <c r="G962" s="14"/>
-      <c r="H962" s="14"/>
-      <c r="I962" s="14"/>
-      <c r="J962" s="14"/>
-      <c r="K962" s="14"/>
-      <c r="L962" s="14"/>
-      <c r="M962" s="14"/>
-      <c r="N962" s="14"/>
-      <c r="O962" s="14"/>
-      <c r="P962" s="14"/>
-      <c r="Q962" s="14"/>
-      <c r="R962" s="14"/>
-      <c r="S962" s="14"/>
-      <c r="T962" s="14"/>
-      <c r="U962" s="14"/>
-      <c r="V962" s="14"/>
-      <c r="W962" s="14"/>
-      <c r="X962" s="14"/>
-      <c r="Y962" s="14"/>
-      <c r="Z962" s="14"/>
-    </row>
-    <row r="963" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A963" s="12"/>
-      <c r="B963" s="13"/>
-      <c r="C963" s="12"/>
-      <c r="D963" s="14"/>
-      <c r="E963" s="14"/>
-      <c r="F963" s="14"/>
-      <c r="G963" s="14"/>
-      <c r="H963" s="14"/>
-      <c r="I963" s="14"/>
-      <c r="J963" s="14"/>
-      <c r="K963" s="14"/>
-      <c r="L963" s="14"/>
-      <c r="M963" s="14"/>
-      <c r="N963" s="14"/>
-      <c r="O963" s="14"/>
-      <c r="P963" s="14"/>
-      <c r="Q963" s="14"/>
-      <c r="R963" s="14"/>
-      <c r="S963" s="14"/>
-      <c r="T963" s="14"/>
-      <c r="U963" s="14"/>
-      <c r="V963" s="14"/>
-      <c r="W963" s="14"/>
-      <c r="X963" s="14"/>
-      <c r="Y963" s="14"/>
-      <c r="Z963" s="14"/>
-    </row>
-    <row r="964" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A964" s="12"/>
-      <c r="B964" s="13"/>
-      <c r="C964" s="12"/>
-      <c r="D964" s="14"/>
-      <c r="E964" s="14"/>
-      <c r="F964" s="14"/>
-      <c r="G964" s="14"/>
-      <c r="H964" s="14"/>
-      <c r="I964" s="14"/>
-      <c r="J964" s="14"/>
-      <c r="K964" s="14"/>
-      <c r="L964" s="14"/>
-      <c r="M964" s="14"/>
-      <c r="N964" s="14"/>
-      <c r="O964" s="14"/>
-      <c r="P964" s="14"/>
-      <c r="Q964" s="14"/>
-      <c r="R964" s="14"/>
-      <c r="S964" s="14"/>
-      <c r="T964" s="14"/>
-      <c r="U964" s="14"/>
-      <c r="V964" s="14"/>
-      <c r="W964" s="14"/>
-      <c r="X964" s="14"/>
-      <c r="Y964" s="14"/>
-      <c r="Z964" s="14"/>
-    </row>
-    <row r="965" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A965" s="12"/>
-      <c r="B965" s="13"/>
-      <c r="C965" s="12"/>
-      <c r="D965" s="14"/>
-      <c r="E965" s="14"/>
-      <c r="F965" s="14"/>
-      <c r="G965" s="14"/>
-      <c r="H965" s="14"/>
-      <c r="I965" s="14"/>
-      <c r="J965" s="14"/>
-      <c r="K965" s="14"/>
-      <c r="L965" s="14"/>
-      <c r="M965" s="14"/>
-      <c r="N965" s="14"/>
-      <c r="O965" s="14"/>
-      <c r="P965" s="14"/>
-      <c r="Q965" s="14"/>
-      <c r="R965" s="14"/>
-      <c r="S965" s="14"/>
-      <c r="T965" s="14"/>
-      <c r="U965" s="14"/>
-      <c r="V965" s="14"/>
-      <c r="W965" s="14"/>
-      <c r="X965" s="14"/>
-      <c r="Y965" s="14"/>
-      <c r="Z965" s="14"/>
-    </row>
-    <row r="966" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A966" s="12"/>
-      <c r="B966" s="13"/>
-      <c r="C966" s="12"/>
-      <c r="D966" s="14"/>
-      <c r="E966" s="14"/>
-      <c r="F966" s="14"/>
-      <c r="G966" s="14"/>
-      <c r="H966" s="14"/>
-      <c r="I966" s="14"/>
-      <c r="J966" s="14"/>
-      <c r="K966" s="14"/>
-      <c r="L966" s="14"/>
-      <c r="M966" s="14"/>
-      <c r="N966" s="14"/>
-      <c r="O966" s="14"/>
-      <c r="P966" s="14"/>
-      <c r="Q966" s="14"/>
-      <c r="R966" s="14"/>
-      <c r="S966" s="14"/>
-      <c r="T966" s="14"/>
-      <c r="U966" s="14"/>
-      <c r="V966" s="14"/>
-      <c r="W966" s="14"/>
-      <c r="X966" s="14"/>
-      <c r="Y966" s="14"/>
-      <c r="Z966" s="14"/>
-    </row>
-    <row r="967" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A967" s="12"/>
-      <c r="B967" s="13"/>
-      <c r="C967" s="12"/>
-      <c r="D967" s="14"/>
-      <c r="E967" s="14"/>
-      <c r="F967" s="14"/>
-      <c r="G967" s="14"/>
-      <c r="H967" s="14"/>
-      <c r="I967" s="14"/>
-      <c r="J967" s="14"/>
-      <c r="K967" s="14"/>
-      <c r="L967" s="14"/>
-      <c r="M967" s="14"/>
-      <c r="N967" s="14"/>
-      <c r="O967" s="14"/>
-      <c r="P967" s="14"/>
-      <c r="Q967" s="14"/>
-      <c r="R967" s="14"/>
-      <c r="S967" s="14"/>
-      <c r="T967" s="14"/>
-      <c r="U967" s="14"/>
-      <c r="V967" s="14"/>
-      <c r="W967" s="14"/>
-      <c r="X967" s="14"/>
-      <c r="Y967" s="14"/>
-      <c r="Z967" s="14"/>
-    </row>
-    <row r="968" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A968" s="12"/>
-      <c r="B968" s="13"/>
-      <c r="C968" s="12"/>
-      <c r="D968" s="14"/>
-      <c r="E968" s="14"/>
-      <c r="F968" s="14"/>
-      <c r="G968" s="14"/>
-      <c r="H968" s="14"/>
-      <c r="I968" s="14"/>
-      <c r="J968" s="14"/>
-      <c r="K968" s="14"/>
-      <c r="L968" s="14"/>
-      <c r="M968" s="14"/>
-      <c r="N968" s="14"/>
-      <c r="O968" s="14"/>
-      <c r="P968" s="14"/>
-      <c r="Q968" s="14"/>
-      <c r="R968" s="14"/>
-      <c r="S968" s="14"/>
-      <c r="T968" s="14"/>
-      <c r="U968" s="14"/>
-      <c r="V968" s="14"/>
-      <c r="W968" s="14"/>
-      <c r="X968" s="14"/>
-      <c r="Y968" s="14"/>
-      <c r="Z968" s="14"/>
-    </row>
-    <row r="969" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A969" s="12"/>
-      <c r="B969" s="13"/>
-      <c r="C969" s="12"/>
-      <c r="D969" s="14"/>
-      <c r="E969" s="14"/>
-      <c r="F969" s="14"/>
-      <c r="G969" s="14"/>
-      <c r="H969" s="14"/>
-      <c r="I969" s="14"/>
-      <c r="J969" s="14"/>
-      <c r="K969" s="14"/>
-      <c r="L969" s="14"/>
-      <c r="M969" s="14"/>
-      <c r="N969" s="14"/>
-      <c r="O969" s="14"/>
-      <c r="P969" s="14"/>
-      <c r="Q969" s="14"/>
-      <c r="R969" s="14"/>
-      <c r="S969" s="14"/>
-      <c r="T969" s="14"/>
-      <c r="U969" s="14"/>
-      <c r="V969" s="14"/>
-      <c r="W969" s="14"/>
-      <c r="X969" s="14"/>
-      <c r="Y969" s="14"/>
-      <c r="Z969" s="14"/>
-    </row>
-    <row r="970" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A970" s="12"/>
-      <c r="B970" s="13"/>
-      <c r="C970" s="12"/>
-      <c r="D970" s="14"/>
-      <c r="E970" s="14"/>
-      <c r="F970" s="14"/>
-      <c r="G970" s="14"/>
-      <c r="H970" s="14"/>
-      <c r="I970" s="14"/>
-      <c r="J970" s="14"/>
-      <c r="K970" s="14"/>
-      <c r="L970" s="14"/>
-      <c r="M970" s="14"/>
-      <c r="N970" s="14"/>
-      <c r="O970" s="14"/>
-      <c r="P970" s="14"/>
-      <c r="Q970" s="14"/>
-      <c r="R970" s="14"/>
-      <c r="S970" s="14"/>
-      <c r="T970" s="14"/>
-      <c r="U970" s="14"/>
-      <c r="V970" s="14"/>
-      <c r="W970" s="14"/>
-      <c r="X970" s="14"/>
-      <c r="Y970" s="14"/>
-      <c r="Z970" s="14"/>
-    </row>
-    <row r="971" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A971" s="12"/>
-      <c r="B971" s="13"/>
-      <c r="C971" s="12"/>
-      <c r="D971" s="14"/>
-      <c r="E971" s="14"/>
-      <c r="F971" s="14"/>
-      <c r="G971" s="14"/>
-      <c r="H971" s="14"/>
-      <c r="I971" s="14"/>
-      <c r="J971" s="14"/>
-      <c r="K971" s="14"/>
-      <c r="L971" s="14"/>
-      <c r="M971" s="14"/>
-      <c r="N971" s="14"/>
-      <c r="O971" s="14"/>
-      <c r="P971" s="14"/>
-      <c r="Q971" s="14"/>
-      <c r="R971" s="14"/>
-      <c r="S971" s="14"/>
-      <c r="T971" s="14"/>
-      <c r="U971" s="14"/>
-      <c r="V971" s="14"/>
-      <c r="W971" s="14"/>
-      <c r="X971" s="14"/>
-      <c r="Y971" s="14"/>
-      <c r="Z971" s="14"/>
-    </row>
-    <row r="972" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A972" s="12"/>
-      <c r="B972" s="13"/>
-      <c r="C972" s="12"/>
-      <c r="D972" s="14"/>
-      <c r="E972" s="14"/>
-      <c r="F972" s="14"/>
-      <c r="G972" s="14"/>
-      <c r="H972" s="14"/>
-      <c r="I972" s="14"/>
-      <c r="J972" s="14"/>
-      <c r="K972" s="14"/>
-      <c r="L972" s="14"/>
-      <c r="M972" s="14"/>
-      <c r="N972" s="14"/>
-      <c r="O972" s="14"/>
-      <c r="P972" s="14"/>
-      <c r="Q972" s="14"/>
-      <c r="R972" s="14"/>
-      <c r="S972" s="14"/>
-      <c r="T972" s="14"/>
-      <c r="U972" s="14"/>
-      <c r="V972" s="14"/>
-      <c r="W972" s="14"/>
-      <c r="X972" s="14"/>
-      <c r="Y972" s="14"/>
-      <c r="Z972" s="14"/>
-    </row>
-    <row r="973" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A973" s="12"/>
-      <c r="B973" s="13"/>
-      <c r="C973" s="12"/>
-      <c r="D973" s="14"/>
-      <c r="E973" s="14"/>
-      <c r="F973" s="14"/>
-      <c r="G973" s="14"/>
-      <c r="H973" s="14"/>
-      <c r="I973" s="14"/>
-      <c r="J973" s="14"/>
-      <c r="K973" s="14"/>
-      <c r="L973" s="14"/>
-      <c r="M973" s="14"/>
-      <c r="N973" s="14"/>
-      <c r="O973" s="14"/>
-      <c r="P973" s="14"/>
-      <c r="Q973" s="14"/>
-      <c r="R973" s="14"/>
-      <c r="S973" s="14"/>
-      <c r="T973" s="14"/>
-      <c r="U973" s="14"/>
-      <c r="V973" s="14"/>
-      <c r="W973" s="14"/>
-      <c r="X973" s="14"/>
-      <c r="Y973" s="14"/>
-      <c r="Z973" s="14"/>
-    </row>
-    <row r="974" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A974" s="12"/>
-      <c r="B974" s="13"/>
-      <c r="C974" s="12"/>
-      <c r="D974" s="14"/>
-      <c r="E974" s="14"/>
-      <c r="F974" s="14"/>
-      <c r="G974" s="14"/>
-      <c r="H974" s="14"/>
-      <c r="I974" s="14"/>
-      <c r="J974" s="14"/>
-      <c r="K974" s="14"/>
-      <c r="L974" s="14"/>
-      <c r="M974" s="14"/>
-      <c r="N974" s="14"/>
-      <c r="O974" s="14"/>
-      <c r="P974" s="14"/>
-      <c r="Q974" s="14"/>
-      <c r="R974" s="14"/>
-      <c r="S974" s="14"/>
-      <c r="T974" s="14"/>
-      <c r="U974" s="14"/>
-      <c r="V974" s="14"/>
-      <c r="W974" s="14"/>
-      <c r="X974" s="14"/>
-      <c r="Y974" s="14"/>
-      <c r="Z974" s="14"/>
-    </row>
-    <row r="975" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A975" s="12"/>
-      <c r="B975" s="13"/>
-      <c r="C975" s="12"/>
-      <c r="D975" s="14"/>
-      <c r="E975" s="14"/>
-      <c r="F975" s="14"/>
-      <c r="G975" s="14"/>
-      <c r="H975" s="14"/>
-      <c r="I975" s="14"/>
-      <c r="J975" s="14"/>
-      <c r="K975" s="14"/>
-      <c r="L975" s="14"/>
-      <c r="M975" s="14"/>
-      <c r="N975" s="14"/>
-      <c r="O975" s="14"/>
-      <c r="P975" s="14"/>
-      <c r="Q975" s="14"/>
-      <c r="R975" s="14"/>
-      <c r="S975" s="14"/>
-      <c r="T975" s="14"/>
-      <c r="U975" s="14"/>
-      <c r="V975" s="14"/>
-      <c r="W975" s="14"/>
-      <c r="X975" s="14"/>
-      <c r="Y975" s="14"/>
-      <c r="Z975" s="14"/>
-    </row>
-    <row r="976" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A976" s="12"/>
-      <c r="B976" s="13"/>
-      <c r="C976" s="12"/>
-      <c r="D976" s="14"/>
-      <c r="E976" s="14"/>
-      <c r="F976" s="14"/>
-      <c r="G976" s="14"/>
-      <c r="H976" s="14"/>
-      <c r="I976" s="14"/>
-      <c r="J976" s="14"/>
-      <c r="K976" s="14"/>
-      <c r="L976" s="14"/>
-      <c r="M976" s="14"/>
-      <c r="N976" s="14"/>
-      <c r="O976" s="14"/>
-      <c r="P976" s="14"/>
-      <c r="Q976" s="14"/>
-      <c r="R976" s="14"/>
-      <c r="S976" s="14"/>
-      <c r="T976" s="14"/>
-      <c r="U976" s="14"/>
-      <c r="V976" s="14"/>
-      <c r="W976" s="14"/>
-      <c r="X976" s="14"/>
-      <c r="Y976" s="14"/>
-      <c r="Z976" s="14"/>
-    </row>
-    <row r="977" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A977" s="12"/>
-      <c r="B977" s="13"/>
-      <c r="C977" s="12"/>
-      <c r="D977" s="14"/>
-      <c r="E977" s="14"/>
-      <c r="F977" s="14"/>
-      <c r="G977" s="14"/>
-      <c r="H977" s="14"/>
-      <c r="I977" s="14"/>
-      <c r="J977" s="14"/>
-      <c r="K977" s="14"/>
-      <c r="L977" s="14"/>
-      <c r="M977" s="14"/>
-      <c r="N977" s="14"/>
-      <c r="O977" s="14"/>
-      <c r="P977" s="14"/>
-      <c r="Q977" s="14"/>
-      <c r="R977" s="14"/>
-      <c r="S977" s="14"/>
-      <c r="T977" s="14"/>
-      <c r="U977" s="14"/>
-      <c r="V977" s="14"/>
-      <c r="W977" s="14"/>
-      <c r="X977" s="14"/>
-      <c r="Y977" s="14"/>
-      <c r="Z977" s="14"/>
-    </row>
-    <row r="978" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A978" s="12"/>
-      <c r="B978" s="13"/>
-      <c r="C978" s="12"/>
-      <c r="D978" s="14"/>
-      <c r="E978" s="14"/>
-      <c r="F978" s="14"/>
-      <c r="G978" s="14"/>
-      <c r="H978" s="14"/>
-      <c r="I978" s="14"/>
-      <c r="J978" s="14"/>
-      <c r="K978" s="14"/>
-      <c r="L978" s="14"/>
-      <c r="M978" s="14"/>
-      <c r="N978" s="14"/>
-      <c r="O978" s="14"/>
-      <c r="P978" s="14"/>
-      <c r="Q978" s="14"/>
-      <c r="R978" s="14"/>
-      <c r="S978" s="14"/>
-      <c r="T978" s="14"/>
-      <c r="U978" s="14"/>
-      <c r="V978" s="14"/>
-      <c r="W978" s="14"/>
-      <c r="X978" s="14"/>
-      <c r="Y978" s="14"/>
-      <c r="Z978" s="14"/>
-    </row>
-    <row r="979" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A979" s="12"/>
-      <c r="B979" s="13"/>
-      <c r="C979" s="12"/>
-      <c r="D979" s="14"/>
-      <c r="E979" s="14"/>
-      <c r="F979" s="14"/>
-      <c r="G979" s="14"/>
-      <c r="H979" s="14"/>
-      <c r="I979" s="14"/>
-      <c r="J979" s="14"/>
-      <c r="K979" s="14"/>
-      <c r="L979" s="14"/>
-      <c r="M979" s="14"/>
-      <c r="N979" s="14"/>
-      <c r="O979" s="14"/>
-      <c r="P979" s="14"/>
-      <c r="Q979" s="14"/>
-      <c r="R979" s="14"/>
-      <c r="S979" s="14"/>
-      <c r="T979" s="14"/>
-      <c r="U979" s="14"/>
-      <c r="V979" s="14"/>
-      <c r="W979" s="14"/>
-      <c r="X979" s="14"/>
-      <c r="Y979" s="14"/>
-      <c r="Z979" s="14"/>
-    </row>
-    <row r="980" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A980" s="12"/>
-      <c r="B980" s="13"/>
-      <c r="C980" s="12"/>
-      <c r="D980" s="14"/>
-      <c r="E980" s="14"/>
-      <c r="F980" s="14"/>
-      <c r="G980" s="14"/>
-      <c r="H980" s="14"/>
-      <c r="I980" s="14"/>
-      <c r="J980" s="14"/>
-      <c r="K980" s="14"/>
-      <c r="L980" s="14"/>
-      <c r="M980" s="14"/>
-      <c r="N980" s="14"/>
-      <c r="O980" s="14"/>
-      <c r="P980" s="14"/>
-      <c r="Q980" s="14"/>
-      <c r="R980" s="14"/>
-      <c r="S980" s="14"/>
-      <c r="T980" s="14"/>
-      <c r="U980" s="14"/>
-      <c r="V980" s="14"/>
-      <c r="W980" s="14"/>
-      <c r="X980" s="14"/>
-      <c r="Y980" s="14"/>
-      <c r="Z980" s="14"/>
-    </row>
-    <row r="981" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A981" s="12"/>
-      <c r="B981" s="13"/>
-      <c r="C981" s="12"/>
-      <c r="D981" s="14"/>
-      <c r="E981" s="14"/>
-      <c r="F981" s="14"/>
-      <c r="G981" s="14"/>
-      <c r="H981" s="14"/>
-      <c r="I981" s="14"/>
-      <c r="J981" s="14"/>
-      <c r="K981" s="14"/>
-      <c r="L981" s="14"/>
-      <c r="M981" s="14"/>
-      <c r="N981" s="14"/>
-      <c r="O981" s="14"/>
-      <c r="P981" s="14"/>
-      <c r="Q981" s="14"/>
-      <c r="R981" s="14"/>
-      <c r="S981" s="14"/>
-      <c r="T981" s="14"/>
-      <c r="U981" s="14"/>
-      <c r="V981" s="14"/>
-      <c r="W981" s="14"/>
-      <c r="X981" s="14"/>
-      <c r="Y981" s="14"/>
-      <c r="Z981" s="14"/>
-    </row>
-    <row r="982" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A982" s="12"/>
-      <c r="B982" s="13"/>
-      <c r="C982" s="12"/>
-      <c r="D982" s="14"/>
-      <c r="E982" s="14"/>
-      <c r="F982" s="14"/>
-      <c r="G982" s="14"/>
-      <c r="H982" s="14"/>
-      <c r="I982" s="14"/>
-      <c r="J982" s="14"/>
-      <c r="K982" s="14"/>
-      <c r="L982" s="14"/>
-      <c r="M982" s="14"/>
-      <c r="N982" s="14"/>
-      <c r="O982" s="14"/>
-      <c r="P982" s="14"/>
-      <c r="Q982" s="14"/>
-      <c r="R982" s="14"/>
-      <c r="S982" s="14"/>
-      <c r="T982" s="14"/>
-      <c r="U982" s="14"/>
-      <c r="V982" s="14"/>
-      <c r="W982" s="14"/>
-      <c r="X982" s="14"/>
-      <c r="Y982" s="14"/>
-      <c r="Z982" s="14"/>
-    </row>
-    <row r="983" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A983" s="12"/>
-      <c r="B983" s="13"/>
-      <c r="C983" s="12"/>
-      <c r="D983" s="14"/>
-      <c r="E983" s="14"/>
-      <c r="F983" s="14"/>
-      <c r="G983" s="14"/>
-      <c r="H983" s="14"/>
-      <c r="I983" s="14"/>
-      <c r="J983" s="14"/>
-      <c r="K983" s="14"/>
-      <c r="L983" s="14"/>
-      <c r="M983" s="14"/>
-      <c r="N983" s="14"/>
-      <c r="O983" s="14"/>
-      <c r="P983" s="14"/>
-      <c r="Q983" s="14"/>
-      <c r="R983" s="14"/>
-      <c r="S983" s="14"/>
-      <c r="T983" s="14"/>
-      <c r="U983" s="14"/>
-      <c r="V983" s="14"/>
-      <c r="W983" s="14"/>
-      <c r="X983" s="14"/>
-      <c r="Y983" s="14"/>
-      <c r="Z983" s="14"/>
-    </row>
-    <row r="984" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A984" s="12"/>
-      <c r="B984" s="13"/>
-      <c r="C984" s="12"/>
-      <c r="D984" s="14"/>
-      <c r="E984" s="14"/>
-      <c r="F984" s="14"/>
-      <c r="G984" s="14"/>
-      <c r="H984" s="14"/>
-      <c r="I984" s="14"/>
-      <c r="J984" s="14"/>
-      <c r="K984" s="14"/>
-      <c r="L984" s="14"/>
-      <c r="M984" s="14"/>
-      <c r="N984" s="14"/>
-      <c r="O984" s="14"/>
-      <c r="P984" s="14"/>
-      <c r="Q984" s="14"/>
-      <c r="R984" s="14"/>
-      <c r="S984" s="14"/>
-      <c r="T984" s="14"/>
-      <c r="U984" s="14"/>
-      <c r="V984" s="14"/>
-      <c r="W984" s="14"/>
-      <c r="X984" s="14"/>
-      <c r="Y984" s="14"/>
-      <c r="Z984" s="14"/>
-    </row>
-    <row r="985" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A985" s="12"/>
-      <c r="B985" s="13"/>
-      <c r="C985" s="12"/>
-      <c r="D985" s="14"/>
-      <c r="E985" s="14"/>
-      <c r="F985" s="14"/>
-      <c r="G985" s="14"/>
-      <c r="H985" s="14"/>
-      <c r="I985" s="14"/>
-      <c r="J985" s="14"/>
-      <c r="K985" s="14"/>
-      <c r="L985" s="14"/>
-      <c r="M985" s="14"/>
-      <c r="N985" s="14"/>
-      <c r="O985" s="14"/>
-      <c r="P985" s="14"/>
-      <c r="Q985" s="14"/>
-      <c r="R985" s="14"/>
-      <c r="S985" s="14"/>
-      <c r="T985" s="14"/>
-      <c r="U985" s="14"/>
-      <c r="V985" s="14"/>
-      <c r="W985" s="14"/>
-      <c r="X985" s="14"/>
-      <c r="Y985" s="14"/>
-      <c r="Z985" s="14"/>
-    </row>
-    <row r="986" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A986" s="12"/>
-      <c r="B986" s="13"/>
-      <c r="C986" s="12"/>
-      <c r="D986" s="14"/>
-      <c r="E986" s="14"/>
-      <c r="F986" s="14"/>
-      <c r="G986" s="14"/>
-      <c r="H986" s="14"/>
-      <c r="I986" s="14"/>
-      <c r="J986" s="14"/>
-      <c r="K986" s="14"/>
-      <c r="L986" s="14"/>
-      <c r="M986" s="14"/>
-      <c r="N986" s="14"/>
-      <c r="O986" s="14"/>
-      <c r="P986" s="14"/>
-      <c r="Q986" s="14"/>
-      <c r="R986" s="14"/>
-      <c r="S986" s="14"/>
-      <c r="T986" s="14"/>
-      <c r="U986" s="14"/>
-      <c r="V986" s="14"/>
-      <c r="W986" s="14"/>
-      <c r="X986" s="14"/>
-      <c r="Y986" s="14"/>
-      <c r="Z986" s="14"/>
-    </row>
-    <row r="987" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A987" s="12"/>
-      <c r="B987" s="13"/>
-      <c r="C987" s="12"/>
-      <c r="D987" s="14"/>
-      <c r="E987" s="14"/>
-      <c r="F987" s="14"/>
-      <c r="G987" s="14"/>
-      <c r="H987" s="14"/>
-      <c r="I987" s="14"/>
-      <c r="J987" s="14"/>
-      <c r="K987" s="14"/>
-      <c r="L987" s="14"/>
-      <c r="M987" s="14"/>
-      <c r="N987" s="14"/>
-      <c r="O987" s="14"/>
-      <c r="P987" s="14"/>
-      <c r="Q987" s="14"/>
-      <c r="R987" s="14"/>
-      <c r="S987" s="14"/>
-      <c r="T987" s="14"/>
-      <c r="U987" s="14"/>
-      <c r="V987" s="14"/>
-      <c r="W987" s="14"/>
-      <c r="X987" s="14"/>
-      <c r="Y987" s="14"/>
-      <c r="Z987" s="14"/>
-    </row>
-    <row r="988" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A988" s="12"/>
-      <c r="B988" s="13"/>
-      <c r="C988" s="12"/>
-      <c r="D988" s="14"/>
-      <c r="E988" s="14"/>
-      <c r="F988" s="14"/>
-      <c r="G988" s="14"/>
-      <c r="H988" s="14"/>
-      <c r="I988" s="14"/>
-      <c r="J988" s="14"/>
-      <c r="K988" s="14"/>
-      <c r="L988" s="14"/>
-      <c r="M988" s="14"/>
-      <c r="N988" s="14"/>
-      <c r="O988" s="14"/>
-      <c r="P988" s="14"/>
-      <c r="Q988" s="14"/>
-      <c r="R988" s="14"/>
-      <c r="S988" s="14"/>
-      <c r="T988" s="14"/>
-      <c r="U988" s="14"/>
-      <c r="V988" s="14"/>
-      <c r="W988" s="14"/>
-      <c r="X988" s="14"/>
-      <c r="Y988" s="14"/>
-      <c r="Z988" s="14"/>
-    </row>
-    <row r="989" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A989" s="12"/>
-      <c r="B989" s="13"/>
-      <c r="C989" s="12"/>
-      <c r="D989" s="14"/>
-      <c r="E989" s="14"/>
-      <c r="F989" s="14"/>
-      <c r="G989" s="14"/>
-      <c r="H989" s="14"/>
-      <c r="I989" s="14"/>
-      <c r="J989" s="14"/>
-      <c r="K989" s="14"/>
-      <c r="L989" s="14"/>
-      <c r="M989" s="14"/>
-      <c r="N989" s="14"/>
-      <c r="O989" s="14"/>
-      <c r="P989" s="14"/>
-      <c r="Q989" s="14"/>
-      <c r="R989" s="14"/>
-      <c r="S989" s="14"/>
-      <c r="T989" s="14"/>
-      <c r="U989" s="14"/>
-      <c r="V989" s="14"/>
-      <c r="W989" s="14"/>
-      <c r="X989" s="14"/>
-      <c r="Y989" s="14"/>
-      <c r="Z989" s="14"/>
-    </row>
-    <row r="990" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A990" s="12"/>
-      <c r="B990" s="13"/>
-      <c r="C990" s="12"/>
-      <c r="D990" s="14"/>
-      <c r="E990" s="14"/>
-      <c r="F990" s="14"/>
-      <c r="G990" s="14"/>
-      <c r="H990" s="14"/>
-      <c r="I990" s="14"/>
-      <c r="J990" s="14"/>
-      <c r="K990" s="14"/>
-      <c r="L990" s="14"/>
-      <c r="M990" s="14"/>
-      <c r="N990" s="14"/>
-      <c r="O990" s="14"/>
-      <c r="P990" s="14"/>
-      <c r="Q990" s="14"/>
-      <c r="R990" s="14"/>
-      <c r="S990" s="14"/>
-      <c r="T990" s="14"/>
-      <c r="U990" s="14"/>
-      <c r="V990" s="14"/>
-      <c r="W990" s="14"/>
-      <c r="X990" s="14"/>
-      <c r="Y990" s="14"/>
-      <c r="Z990" s="14"/>
-    </row>
-    <row r="991" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A991" s="12"/>
-      <c r="B991" s="13"/>
-      <c r="C991" s="12"/>
-      <c r="D991" s="14"/>
-      <c r="E991" s="14"/>
-      <c r="F991" s="14"/>
-      <c r="G991" s="14"/>
-      <c r="H991" s="14"/>
-      <c r="I991" s="14"/>
-      <c r="J991" s="14"/>
-      <c r="K991" s="14"/>
-      <c r="L991" s="14"/>
-      <c r="M991" s="14"/>
-      <c r="N991" s="14"/>
-      <c r="O991" s="14"/>
-      <c r="P991" s="14"/>
-      <c r="Q991" s="14"/>
-      <c r="R991" s="14"/>
-      <c r="S991" s="14"/>
-      <c r="T991" s="14"/>
-      <c r="U991" s="14"/>
-      <c r="V991" s="14"/>
-      <c r="W991" s="14"/>
-      <c r="X991" s="14"/>
-      <c r="Y991" s="14"/>
-      <c r="Z991" s="14"/>
-    </row>
-    <row r="992" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A992" s="12"/>
-      <c r="B992" s="13"/>
-      <c r="C992" s="12"/>
-      <c r="D992" s="14"/>
-      <c r="E992" s="14"/>
-      <c r="F992" s="14"/>
-      <c r="G992" s="14"/>
-      <c r="H992" s="14"/>
-      <c r="I992" s="14"/>
-      <c r="J992" s="14"/>
-      <c r="K992" s="14"/>
-      <c r="L992" s="14"/>
-      <c r="M992" s="14"/>
-      <c r="N992" s="14"/>
-      <c r="O992" s="14"/>
-      <c r="P992" s="14"/>
-      <c r="Q992" s="14"/>
-      <c r="R992" s="14"/>
-      <c r="S992" s="14"/>
-      <c r="T992" s="14"/>
-      <c r="U992" s="14"/>
-      <c r="V992" s="14"/>
-      <c r="W992" s="14"/>
-      <c r="X992" s="14"/>
-      <c r="Y992" s="14"/>
-      <c r="Z992" s="14"/>
-    </row>
-    <row r="993" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A993" s="12"/>
-      <c r="B993" s="13"/>
-      <c r="C993" s="12"/>
-      <c r="D993" s="14"/>
-      <c r="E993" s="14"/>
-      <c r="F993" s="14"/>
-      <c r="G993" s="14"/>
-      <c r="H993" s="14"/>
-      <c r="I993" s="14"/>
-      <c r="J993" s="14"/>
-      <c r="K993" s="14"/>
-      <c r="L993" s="14"/>
-      <c r="M993" s="14"/>
-      <c r="N993" s="14"/>
-      <c r="O993" s="14"/>
-      <c r="P993" s="14"/>
-      <c r="Q993" s="14"/>
-      <c r="R993" s="14"/>
-      <c r="S993" s="14"/>
-      <c r="T993" s="14"/>
-      <c r="U993" s="14"/>
-      <c r="V993" s="14"/>
-      <c r="W993" s="14"/>
-      <c r="X993" s="14"/>
-      <c r="Y993" s="14"/>
-      <c r="Z993" s="14"/>
-    </row>
-    <row r="994" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A994" s="12"/>
-      <c r="B994" s="13"/>
-      <c r="C994" s="12"/>
-      <c r="D994" s="14"/>
-      <c r="E994" s="14"/>
-      <c r="F994" s="14"/>
-      <c r="G994" s="14"/>
-      <c r="H994" s="14"/>
-      <c r="I994" s="14"/>
-      <c r="J994" s="14"/>
-      <c r="K994" s="14"/>
-      <c r="L994" s="14"/>
-      <c r="M994" s="14"/>
-      <c r="N994" s="14"/>
-      <c r="O994" s="14"/>
-      <c r="P994" s="14"/>
-      <c r="Q994" s="14"/>
-      <c r="R994" s="14"/>
-      <c r="S994" s="14"/>
-      <c r="T994" s="14"/>
-      <c r="U994" s="14"/>
-      <c r="V994" s="14"/>
-      <c r="W994" s="14"/>
-      <c r="X994" s="14"/>
-      <c r="Y994" s="14"/>
-      <c r="Z994" s="14"/>
-    </row>
-    <row r="995" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A995" s="12"/>
-      <c r="B995" s="13"/>
-      <c r="C995" s="12"/>
-      <c r="D995" s="14"/>
-      <c r="E995" s="14"/>
-      <c r="F995" s="14"/>
-      <c r="G995" s="14"/>
-      <c r="H995" s="14"/>
-      <c r="I995" s="14"/>
-      <c r="J995" s="14"/>
-      <c r="K995" s="14"/>
-      <c r="L995" s="14"/>
-      <c r="M995" s="14"/>
-      <c r="N995" s="14"/>
-      <c r="O995" s="14"/>
-      <c r="P995" s="14"/>
-      <c r="Q995" s="14"/>
-      <c r="R995" s="14"/>
-      <c r="S995" s="14"/>
-      <c r="T995" s="14"/>
-      <c r="U995" s="14"/>
-      <c r="V995" s="14"/>
-      <c r="W995" s="14"/>
-      <c r="X995" s="14"/>
-      <c r="Y995" s="14"/>
-      <c r="Z995" s="14"/>
-    </row>
-    <row r="996" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A996" s="12"/>
-      <c r="B996" s="13"/>
-      <c r="C996" s="12"/>
-      <c r="D996" s="14"/>
-      <c r="E996" s="14"/>
-      <c r="F996" s="14"/>
-      <c r="G996" s="14"/>
-      <c r="H996" s="14"/>
-      <c r="I996" s="14"/>
-      <c r="J996" s="14"/>
-      <c r="K996" s="14"/>
-      <c r="L996" s="14"/>
-      <c r="M996" s="14"/>
-      <c r="N996" s="14"/>
-      <c r="O996" s="14"/>
-      <c r="P996" s="14"/>
-      <c r="Q996" s="14"/>
-      <c r="R996" s="14"/>
-      <c r="S996" s="14"/>
-      <c r="T996" s="14"/>
-      <c r="U996" s="14"/>
-      <c r="V996" s="14"/>
-      <c r="W996" s="14"/>
-      <c r="X996" s="14"/>
-      <c r="Y996" s="14"/>
-      <c r="Z996" s="14"/>
-    </row>
-    <row r="997" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A997" s="12"/>
-      <c r="B997" s="13"/>
-      <c r="C997" s="12"/>
-      <c r="D997" s="14"/>
-      <c r="E997" s="14"/>
-      <c r="F997" s="14"/>
-      <c r="G997" s="14"/>
-      <c r="H997" s="14"/>
-      <c r="I997" s="14"/>
-      <c r="J997" s="14"/>
-      <c r="K997" s="14"/>
-      <c r="L997" s="14"/>
-      <c r="M997" s="14"/>
-      <c r="N997" s="14"/>
-      <c r="O997" s="14"/>
-      <c r="P997" s="14"/>
-      <c r="Q997" s="14"/>
-      <c r="R997" s="14"/>
-      <c r="S997" s="14"/>
-      <c r="T997" s="14"/>
-      <c r="U997" s="14"/>
-      <c r="V997" s="14"/>
-      <c r="W997" s="14"/>
-      <c r="X997" s="14"/>
-      <c r="Y997" s="14"/>
-      <c r="Z997" s="14"/>
-    </row>
-    <row r="998" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A998" s="12"/>
-      <c r="B998" s="13"/>
-      <c r="C998" s="12"/>
-      <c r="D998" s="14"/>
-      <c r="E998" s="14"/>
-      <c r="F998" s="14"/>
-      <c r="G998" s="14"/>
-      <c r="H998" s="14"/>
-      <c r="I998" s="14"/>
-      <c r="J998" s="14"/>
-      <c r="K998" s="14"/>
-      <c r="L998" s="14"/>
-      <c r="M998" s="14"/>
-      <c r="N998" s="14"/>
-      <c r="O998" s="14"/>
-      <c r="P998" s="14"/>
-      <c r="Q998" s="14"/>
-      <c r="R998" s="14"/>
-      <c r="S998" s="14"/>
-      <c r="T998" s="14"/>
-      <c r="U998" s="14"/>
-      <c r="V998" s="14"/>
-      <c r="W998" s="14"/>
-      <c r="X998" s="14"/>
-      <c r="Y998" s="14"/>
-      <c r="Z998" s="14"/>
-    </row>
-    <row r="999" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A999" s="12"/>
-      <c r="B999" s="13"/>
-      <c r="C999" s="12"/>
-      <c r="D999" s="14"/>
-      <c r="E999" s="14"/>
-      <c r="F999" s="14"/>
-      <c r="G999" s="14"/>
-      <c r="H999" s="14"/>
-      <c r="I999" s="14"/>
-      <c r="J999" s="14"/>
-      <c r="K999" s="14"/>
-      <c r="L999" s="14"/>
-      <c r="M999" s="14"/>
-      <c r="N999" s="14"/>
-      <c r="O999" s="14"/>
-      <c r="P999" s="14"/>
-      <c r="Q999" s="14"/>
-      <c r="R999" s="14"/>
-      <c r="S999" s="14"/>
-      <c r="T999" s="14"/>
-      <c r="U999" s="14"/>
-      <c r="V999" s="14"/>
-      <c r="W999" s="14"/>
-      <c r="X999" s="14"/>
-      <c r="Y999" s="14"/>
-      <c r="Z999" s="14"/>
-    </row>
-    <row r="1000" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1000" s="12"/>
-      <c r="B1000" s="13"/>
-      <c r="C1000" s="12"/>
-      <c r="D1000" s="14"/>
-      <c r="E1000" s="14"/>
-      <c r="F1000" s="14"/>
-      <c r="G1000" s="14"/>
-      <c r="H1000" s="14"/>
-      <c r="I1000" s="14"/>
-      <c r="J1000" s="14"/>
-      <c r="K1000" s="14"/>
-      <c r="L1000" s="14"/>
-      <c r="M1000" s="14"/>
-      <c r="N1000" s="14"/>
-      <c r="O1000" s="14"/>
-      <c r="P1000" s="14"/>
-      <c r="Q1000" s="14"/>
-      <c r="R1000" s="14"/>
-      <c r="S1000" s="14"/>
-      <c r="T1000" s="14"/>
-      <c r="U1000" s="14"/>
-      <c r="V1000" s="14"/>
-      <c r="W1000" s="14"/>
-      <c r="X1000" s="14"/>
-      <c r="Y1000" s="14"/>
-      <c r="Z1000" s="14"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>

</xml_diff>